<commit_message>
test commit for excel
</commit_message>
<xml_diff>
--- a/Team03Report.xlsx
+++ b/Team03Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/937e0d3af198974b/Documents/CS-555/Project/gedcom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="124" documentId="13_ncr:1_{E5D6C071-B4AF-4354-B3D0-F1B91E2B1EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B541A8FA-AEBE-40E3-B45B-D7FDDD68F222}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="13_ncr:1_{E5D6C071-B4AF-4354-B3D0-F1B91E2B1EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E4393C9-1596-4D0C-8BC5-5094F24A8C92}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -581,7 +581,7 @@
     <t>cs555tm032023Fall</t>
   </si>
   <si>
-    <t>ysharma72</t>
+    <t>ysharma</t>
   </si>
 </sst>
 </file>
@@ -1949,7 +1949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -8562,7 +8562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>

</xml_diff>